<commit_message>
added COVID-19 metadata sheets for NGS and microbiology projects and fixes minor typos in regular metadata sheets
</commit_message>
<xml_diff>
--- a/NGS_Metadata_Sheet_1.3.xlsx
+++ b/NGS_Metadata_Sheet_1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marie/Downloads/metadata-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A4B4EC-A0FF-D449-AF43-CB5FB4A5267C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888DEAEA-D269-2947-862C-1285621D8742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,6 +69,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Enter the service description as indicated on the quote for each samples, separate when applicable different services using semicolumn</t>
         </r>
@@ -109,17 +110,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">the ID of the sample on the tube
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(see templates for examples)</t>
+          <t>the ID of the sample on the tube</t>
         </r>
       </text>
     </comment>
@@ -132,7 +123,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>use this column to identify whether the samples belong to the same source (e.g. the same patient (for human) or the same plant (for plants). (see templates for examples)</t>
+          <t>use this column to identify whether the samples belong to the same source (e.g. the same patient (for human) or the same plant (for plants).</t>
         </r>
       </text>
     </comment>
@@ -145,18 +136,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Scientific name of organism(s) from which the biological material was derived.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(see templates for examples) 
-</t>
+          <t>Scientific name of organism(s) from which the biological material was derived.</t>
         </r>
       </text>
     </comment>
@@ -690,7 +670,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -837,11 +817,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1328,6 +1303,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1339,9 +1324,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1358,54 +1340,53 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1415,15 +1396,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1479,44 +1451,47 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2532,44 +2507,44 @@
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="28"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="28"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="E7" s="68" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="E7" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
@@ -2721,38 +2696,38 @@
       </c>
     </row>
     <row r="19" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
     </row>
     <row r="20" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
     </row>
     <row r="21" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
     </row>
     <row r="22" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A22" s="61"/>
@@ -3782,23 +3757,23 @@
       <c r="AMK22" s="62"/>
     </row>
     <row r="23" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="73"/>
+      <c r="B23" s="76"/>
     </row>
     <row r="24" spans="1:1025" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
       <c r="J24" s="62"/>
       <c r="K24" s="62"/>
       <c r="L24" s="62"/>
@@ -4817,15 +4792,15 @@
       <c r="AMK24" s="62"/>
     </row>
     <row r="25" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
       <c r="J25" s="62"/>
       <c r="K25" s="36"/>
       <c r="L25" s="62"/>
@@ -5844,15 +5819,15 @@
       <c r="AMK25" s="62"/>
     </row>
     <row r="26" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A26" s="75"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
       <c r="J26" s="62"/>
       <c r="K26" s="62"/>
       <c r="L26" s="62"/>
@@ -6871,15 +6846,15 @@
       <c r="AMK26" s="62"/>
     </row>
     <row r="27" spans="1:1025" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="75"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
       <c r="J27" s="62"/>
       <c r="K27" s="62"/>
       <c r="L27" s="62"/>
@@ -7898,15 +7873,15 @@
       <c r="AMK27" s="62"/>
     </row>
     <row r="28" spans="1:1025" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="75"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
       <c r="J28" s="62"/>
       <c r="K28" s="62"/>
       <c r="L28" s="62"/>
@@ -8925,15 +8900,15 @@
       <c r="AMK28" s="62"/>
     </row>
     <row r="29" spans="1:1025" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="75"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
       <c r="J29" s="62"/>
       <c r="K29" s="62"/>
       <c r="L29" s="62"/>
@@ -9952,15 +9927,15 @@
       <c r="AMK29" s="62"/>
     </row>
     <row r="30" spans="1:1025" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="75"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
       <c r="J30" s="62"/>
       <c r="K30" s="62"/>
       <c r="L30" s="62"/>
@@ -12006,20 +11981,20 @@
       <c r="AMK31" s="62"/>
     </row>
     <row r="32" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="74"/>
+      <c r="B32" s="77"/>
     </row>
     <row r="33" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
     </row>
     <row r="34" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
@@ -14105,111 +14080,106 @@
       <c r="AMK38" s="62"/>
     </row>
     <row r="39" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A39" s="72" t="s">
+      <c r="A39" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
     </row>
     <row r="40" spans="1:1025" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="69" t="s">
+      <c r="A40" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
     </row>
     <row r="41" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A41" s="70"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
     </row>
     <row r="42" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A42" s="70"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
     </row>
     <row r="44" spans="1:1025" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
       <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B45" s="67"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
       <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B46" s="67"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="71"/>
       <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B47" s="67"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
       <c r="H47" s="37"/>
     </row>
     <row r="48" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B48" s="67"/>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
       <c r="H48" s="37"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="67"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
       <c r="H49" s="37"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="15">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="H5:I6"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:G20"/>
     <mergeCell ref="B44:G49"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
@@ -14220,6 +14190,11 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A24:I30"/>
     <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="H5:I6"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.875" bottom="0.75" header="0.3" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -14256,41 +14231,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="86" t="s">
+      <c r="B1" s="120"/>
+      <c r="C1" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="63"/>
       <c r="B2" s="63"/>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="115" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3" s="64"/>
@@ -14311,69 +14286,69 @@
       <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
       <c r="F6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
       <c r="F7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
       <c r="F8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
       <c r="F9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="124"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
     </row>
     <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -14391,21 +14366,21 @@
       <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -14424,33 +14399,33 @@
       <c r="A19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
     </row>
     <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
     </row>
     <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="113"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="114"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="111"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="113"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="114"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
@@ -14465,8 +14440,8 @@
       <c r="A25" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="106"/>
-      <c r="C25" s="106"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -14477,11 +14452,11 @@
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="108"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
@@ -14492,53 +14467,53 @@
       <c r="A28" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="108" t="s">
+      <c r="B28" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="109"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="111"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="100"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="101"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="94"/>
-      <c r="B30" s="101"/>
-      <c r="C30" s="102"/>
-      <c r="D30" s="102"/>
-      <c r="E30" s="102"/>
-      <c r="F30" s="102"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="103"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="102"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="104"/>
     </row>
     <row r="31" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="96"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="97"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="95"/>
     </row>
     <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
@@ -14549,9 +14524,9 @@
       <c r="A34" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="82"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="119"/>
       <c r="E34" s="57"/>
       <c r="F34" s="57"/>
       <c r="G34" s="57"/>
@@ -14571,67 +14546,67 @@
       <c r="A37" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="114" t="s">
+      <c r="B37" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="115"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="115"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="116"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="82"/>
     </row>
     <row r="38" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="117" t="s">
+      <c r="B38" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="119"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85"/>
     </row>
     <row r="39" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="120" t="s">
+      <c r="A39" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="121" t="s">
+      <c r="B39" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="122"/>
-      <c r="D39" s="122"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="122"/>
-      <c r="G39" s="122"/>
-      <c r="H39" s="123"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="88"/>
+      <c r="H39" s="89"/>
     </row>
     <row r="40" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="120"/>
-      <c r="B40" s="124"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="126"/>
+      <c r="A40" s="86"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="92"/>
     </row>
     <row r="41" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="95" t="s">
+      <c r="B41" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="96"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="96"/>
-      <c r="F41" s="96"/>
-      <c r="G41" s="96"/>
-      <c r="H41" s="97"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="95"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="13"/>
@@ -14674,22 +14649,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B29:H30"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B34:D34"/>
@@ -14706,6 +14665,22 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B29:H30"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:H40"/>
+    <mergeCell ref="B41:H41"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -14736,7 +14711,7 @@
   <dimension ref="A1:AMK502"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>